<commit_message>
Made changes and ran first test run for uncorrected
</commit_message>
<xml_diff>
--- a/data/panel_md_test/samples_md_test.xlsx
+++ b/data/panel_md_test/samples_md_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/testmac/Desktop/gs_pipeline_draft/panel_md_small/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/testmac/Desktop/20250211-BatchCorrect_Comp_Pipeline/data/panel_md_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2AA630-73E2-4146-87A6-6B04DDE39233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2C378A-0CC0-4E42-B3F6-A1216D22BB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="2000" windowWidth="26860" windowHeight="14640" xr2:uid="{6730D803-52B2-684B-B908-D10BD288D371}"/>
+    <workbookView xWindow="1940" yWindow="2000" windowWidth="26860" windowHeight="14640" xr2:uid="{6730D803-52B2-684B-B908-D10BD288D371}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
-    <t>P15_D1_leukocytes.fcs</t>
-  </si>
-  <si>
     <t>file_name</t>
   </si>
   <si>
@@ -62,7 +59,10 @@
     <t>Ctrl</t>
   </si>
   <si>
-    <t>Ctrl_plate1_leukocytes.fcs</t>
+    <t>Ctrl_plate1_leukocytes_test.fcs</t>
+  </si>
+  <si>
+    <t>P15_D1_leukocytes_test.fcs</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,44 +453,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>